<commit_message>
Update Timesheet - Jelte Boumans.xlsx
</commit_message>
<xml_diff>
--- a/Analyse/Timesheet - Jelte Boumans.xlsx
+++ b/Analyse/Timesheet - Jelte Boumans.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jelte\Desktop\Analyse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F77377B-8BCC-438A-BF22-C82FF75724F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{776248B8-9312-4813-88D7-6B56B5CF7BB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -487,8 +487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AG10" sqref="AG10"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AH6" sqref="AH6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,45 +629,39 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>8</v>
-      </c>
-      <c r="C2">
-        <v>8</v>
-      </c>
-      <c r="D2">
-        <v>5</v>
+      <c r="G2">
+        <v>8</v>
+      </c>
+      <c r="H2">
+        <v>8</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="U3">
-        <v>2</v>
-      </c>
       <c r="V3">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="W3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="X3">
         <v>8</v>
       </c>
-      <c r="Y3">
-        <v>8</v>
-      </c>
-      <c r="Z3">
-        <v>8</v>
-      </c>
-      <c r="AA3">
-        <v>8</v>
-      </c>
       <c r="AB3">
         <v>8</v>
       </c>
       <c r="AC3">
+        <v>8</v>
+      </c>
+      <c r="AD3">
+        <v>8</v>
+      </c>
+      <c r="AE3">
         <v>8</v>
       </c>
     </row>
@@ -675,36 +669,12 @@
       <c r="A4" t="s">
         <v>18</v>
       </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="E4">
-        <v>8</v>
-      </c>
-      <c r="F4">
-        <v>8</v>
-      </c>
-      <c r="G4">
-        <v>8</v>
-      </c>
-      <c r="H4">
-        <v>8</v>
-      </c>
       <c r="I4">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J4">
         <v>8</v>
       </c>
-      <c r="K4">
-        <v>8</v>
-      </c>
-      <c r="L4">
-        <v>8</v>
-      </c>
-      <c r="M4">
-        <v>8</v>
-      </c>
       <c r="N4">
         <v>8</v>
       </c>
@@ -717,17 +687,14 @@
       <c r="Q4">
         <v>8</v>
       </c>
-      <c r="R4">
-        <v>8</v>
-      </c>
-      <c r="S4">
-        <v>8</v>
-      </c>
-      <c r="T4">
-        <v>8</v>
-      </c>
       <c r="U4">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="V4">
+        <v>5</v>
+      </c>
+      <c r="W4">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">

</xml_diff>